<commit_message>
Adding some html and images files
</commit_message>
<xml_diff>
--- a/docs/testreadexcel.xlsx
+++ b/docs/testreadexcel.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Repos\Asclepius\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z013jkm/Desktop/Hackathon/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E285F1D-4C2E-F242-A4C6-F664923AA23E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{F4152BB5-5842-F242-AB75-94BB2D8E2C79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,40 +66,40 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Rose</t>
-  </si>
-  <si>
-    <t>Jason</t>
-  </si>
-  <si>
-    <t>Tim</t>
-  </si>
-  <si>
-    <t>Katie</t>
-  </si>
-  <si>
-    <t>Leo</t>
-  </si>
-  <si>
-    <t>Lee</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Luke</t>
-  </si>
-  <si>
-    <t>Chris</t>
+    <t>test data 1</t>
+  </si>
+  <si>
+    <t>test data 2</t>
+  </si>
+  <si>
+    <t>test data 3</t>
+  </si>
+  <si>
+    <t>test data 4</t>
+  </si>
+  <si>
+    <t>test data 5</t>
+  </si>
+  <si>
+    <t>test data 6</t>
+  </si>
+  <si>
+    <t>test data 7</t>
+  </si>
+  <si>
+    <t>test data 8</t>
+  </si>
+  <si>
+    <t>test data 9</t>
+  </si>
+  <si>
+    <t>test data 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -443,19 +444,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C72005-6BA1-C14D-A8F3-526798BBB59B}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -466,7 +467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -477,7 +478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -488,7 +489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -499,7 +500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -510,7 +511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -521,7 +522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -532,7 +533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -543,7 +544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -554,7 +555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -565,7 +566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>

</xml_diff>